<commit_message>
More testing, found good controller with added heading
</commit_message>
<xml_diff>
--- a/Gainsheet.xlsx
+++ b/Gainsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hampu\Documents\Atmel Studio\7.0\AutoBike-Simulation-MDH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD20FE1-DBF3-42DA-9335-3B3363E529BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{189BF987-1A11-4B59-8560-AD1DD4641DB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
   <si>
     <t>I Lat</t>
   </si>
@@ -72,6 +72,9 @@
     <t>Improvement in overshot/turn in</t>
   </si>
   <si>
+    <t>Unstable</t>
+  </si>
+  <si>
     <t>Unstable, flies of course</t>
   </si>
   <si>
@@ -84,10 +87,131 @@
     <t>best</t>
   </si>
   <si>
-    <t>Ostabil</t>
-  </si>
-  <si>
     <t>På med heading</t>
+  </si>
+  <si>
+    <t>bra om man kör med heading</t>
+  </si>
+  <si>
+    <t>No difference when adding derivative</t>
+  </si>
+  <si>
+    <t>Cant go higher</t>
+  </si>
+  <si>
+    <t>Följer hur Path Tracking Control of a Motorcycle
+Based on System Identification gör</t>
+  </si>
+  <si>
+    <t>Unstable after a while</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moves around too much still. </t>
+  </si>
+  <si>
+    <t>180 degrees can increase in error after finnish line</t>
+  </si>
+  <si>
+    <t>While improvements in some areas it have drawbacks over P + P or PD</t>
+  </si>
+  <si>
+    <t>Cant improove with higher gains</t>
+  </si>
+  <si>
+    <t>Combine D with Ph</t>
+  </si>
+  <si>
+    <t>Rally good</t>
+  </si>
+  <si>
+    <t>Workes well</t>
+  </si>
+  <si>
+    <t>Better</t>
+  </si>
+  <si>
+    <t>Tradeoff again</t>
+  </si>
+  <si>
+    <t>---</t>
+  </si>
+  <si>
+    <t>Better way to go</t>
+  </si>
+  <si>
+    <t>How high can we go?</t>
+  </si>
+  <si>
+    <t>sub 1 rrt</t>
+  </si>
+  <si>
+    <t>awsome</t>
+  </si>
+  <si>
+    <t>Shakyness on the straights</t>
+  </si>
+  <si>
+    <t>Tune back from 3.5</t>
+  </si>
+  <si>
+    <t>Smaller shakyness but still there</t>
+  </si>
+  <si>
+    <t>3 seems best</t>
+  </si>
+  <si>
+    <t>Play with derevative</t>
+  </si>
+  <si>
+    <t>Loose a lot of perfromance with less heading</t>
+  </si>
+  <si>
+    <t>Unstable with no heading</t>
+  </si>
+  <si>
+    <t>Can lat D compensate?</t>
+  </si>
+  <si>
+    <t>Still unstable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">More </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stable but not good </t>
+  </si>
+  <si>
+    <t>Unstable again</t>
+  </si>
+  <si>
+    <t>Tune back</t>
+  </si>
+  <si>
+    <t>Not helping</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tuning from 3 again but with D </t>
+  </si>
+  <si>
+    <t>Not as good but less gain</t>
+  </si>
+  <si>
+    <t>How about no D?</t>
+  </si>
+  <si>
+    <t>Little worse. But still good</t>
+  </si>
+  <si>
+    <t>Heading P can compensate?</t>
+  </si>
+  <si>
+    <t>Yes. Better agian</t>
+  </si>
+  <si>
+    <t>Stable still. And better</t>
+  </si>
+  <si>
+    <t>Not as good again</t>
   </si>
 </sst>
 </file>
@@ -123,8 +247,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,15 +533,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
     <col min="9" max="9" width="11.85546875" customWidth="1"/>
     <col min="11" max="11" width="12.5703125" customWidth="1"/>
     <col min="14" max="14" width="43.28515625" customWidth="1"/>
@@ -754,7 +882,7 @@
         <v>14</v>
       </c>
       <c r="O10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -821,7 +949,7 @@
         <v>5.8506341252235003</v>
       </c>
       <c r="N12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -856,7 +984,7 @@
         <v>14.651069710943901</v>
       </c>
       <c r="N13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -891,45 +1019,13 @@
         <v>2.2020890377442299</v>
       </c>
       <c r="N14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>20</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0.5</v>
-      </c>
-      <c r="E15">
-        <v>-0.1</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>1.26276726197713</v>
-      </c>
-      <c r="J15">
-        <v>2.34892935173374E-2</v>
-      </c>
-      <c r="K15">
-        <v>2.6155520163735599</v>
-      </c>
-      <c r="L15">
-        <v>2.1762679985430302</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>1</v>
       </c>
@@ -940,7 +1036,7 @@
         <v>0.5</v>
       </c>
       <c r="E16">
-        <v>-0.2</v>
+        <v>-0.1</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -949,19 +1045,19 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <v>0.94176580644280505</v>
+        <v>1.26276726197713</v>
       </c>
       <c r="J16">
-        <v>1.8034959909606098E-2</v>
+        <v>2.34892935173374E-2</v>
       </c>
       <c r="K16">
-        <v>2.4243504761889301</v>
+        <v>2.6155520163735599</v>
       </c>
       <c r="L16">
-        <v>1.86293162086861</v>
-      </c>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+        <v>2.1762679985430302</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>1</v>
       </c>
@@ -972,7 +1068,7 @@
         <v>0.5</v>
       </c>
       <c r="E17">
-        <v>-0.3</v>
+        <v>-0.2</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -981,24 +1077,21 @@
         <v>0</v>
       </c>
       <c r="I17">
-        <v>4.69963582797123</v>
+        <v>0.94176580644280505</v>
       </c>
       <c r="J17">
-        <v>7.0595638035212502</v>
+        <v>1.8034959909606098E-2</v>
       </c>
       <c r="K17">
-        <v>6.0970818414678298</v>
+        <v>2.4243504761889301</v>
       </c>
       <c r="L17">
-        <v>9.0537006941735108</v>
-      </c>
-      <c r="N17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+        <v>1.86293162086861</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B18">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1007,7 +1100,7 @@
         <v>0.5</v>
       </c>
       <c r="E18">
-        <v>-0.2</v>
+        <v>-0.3</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -1016,19 +1109,22 @@
         <v>0</v>
       </c>
       <c r="I18">
-        <v>0.79793451256500403</v>
+        <v>4.69963582797123</v>
       </c>
       <c r="J18">
-        <v>1.55982113659901E-2</v>
+        <v>7.0595638035212502</v>
       </c>
       <c r="K18">
-        <v>1.97003308090546</v>
+        <v>6.0970818414678298</v>
       </c>
       <c r="L18">
-        <v>1.55603244459863</v>
-      </c>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+        <v>9.0537006941735108</v>
+      </c>
+      <c r="N18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>1.3</v>
       </c>
@@ -1036,7 +1132,7 @@
         <v>0</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E19">
         <v>-0.2</v>
@@ -1048,16 +1144,1242 @@
         <v>0</v>
       </c>
       <c r="I19">
+        <v>0.79793451256500403</v>
+      </c>
+      <c r="J19">
+        <v>1.55982113659901E-2</v>
+      </c>
+      <c r="K19">
+        <v>1.97003308090546</v>
+      </c>
+      <c r="L19">
+        <v>1.55603244459863</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>1.3</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>-0.2</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="I20">
         <v>0.86785510811009303</v>
       </c>
-      <c r="J19">
+      <c r="J20">
         <v>1.6793358125079701E-2</v>
       </c>
-      <c r="K19">
+      <c r="K20">
         <v>2.0058749673020402</v>
       </c>
-      <c r="L19">
+      <c r="L20">
         <v>1.6188860140292101</v>
+      </c>
+      <c r="O20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>1.3</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>-0.2</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0.1</v>
+      </c>
+      <c r="I21">
+        <v>17.046642017401101</v>
+      </c>
+      <c r="J21">
+        <v>18.271472543014202</v>
+      </c>
+      <c r="K21">
+        <v>26.7917828329118</v>
+      </c>
+      <c r="L21">
+        <v>16.394906109117901</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>1.3</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>-0.2</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0.02</v>
+      </c>
+      <c r="I22">
+        <v>0.85416054429949095</v>
+      </c>
+      <c r="J22">
+        <v>1.67262843479925E-2</v>
+      </c>
+      <c r="K22">
+        <v>2.0056978755481398</v>
+      </c>
+      <c r="L22">
+        <v>1.6193762549535</v>
+      </c>
+      <c r="N22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>1.3</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>-0.2</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0.04</v>
+      </c>
+      <c r="I23">
+        <v>6.7527289701147097</v>
+      </c>
+      <c r="J23">
+        <v>6.434619213215</v>
+      </c>
+      <c r="K23">
+        <v>9.0201261145880292</v>
+      </c>
+      <c r="L23">
+        <v>30.9157230367686</v>
+      </c>
+      <c r="N23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>1.3</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>-0.2</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>1.8829624666934599</v>
+      </c>
+      <c r="J25">
+        <v>0.119837161761518</v>
+      </c>
+      <c r="K25">
+        <v>1.1897156796950099</v>
+      </c>
+      <c r="L25">
+        <v>6.1463653193215499</v>
+      </c>
+      <c r="N25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>1.3</v>
+      </c>
+      <c r="C26">
+        <v>0.5</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>-0.2</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>1.28407059496891</v>
+      </c>
+      <c r="J26">
+        <v>3.3754151454153503E-2</v>
+      </c>
+      <c r="K26">
+        <v>0.77561108388869704</v>
+      </c>
+      <c r="L26">
+        <v>2.00956952664079</v>
+      </c>
+      <c r="N26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>1.3</v>
+      </c>
+      <c r="C27">
+        <v>0.2</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>-0.2</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>1.0349645167830199</v>
+      </c>
+      <c r="J27">
+        <v>2.0448902984541901E-2</v>
+      </c>
+      <c r="K27">
+        <v>1.01139294315138</v>
+      </c>
+      <c r="L27">
+        <v>1.4183461138543501</v>
+      </c>
+      <c r="N27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>1.3</v>
+      </c>
+      <c r="C28">
+        <v>0.1</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>-0.2</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0.92562621401170997</v>
+      </c>
+      <c r="J28">
+        <v>1.83550706261137E-2</v>
+      </c>
+      <c r="K28">
+        <v>1.22570984687203</v>
+      </c>
+      <c r="L28">
+        <v>1.6241660782384</v>
+      </c>
+      <c r="N28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>1.6</v>
+      </c>
+      <c r="C29">
+        <v>0.4</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>-0.2</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>1.0938156298363699</v>
+      </c>
+      <c r="J29">
+        <v>2.4955132285744499E-2</v>
+      </c>
+      <c r="K29">
+        <v>0.68326445358298005</v>
+      </c>
+      <c r="L29">
+        <v>1.5721109380312901</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>1.8</v>
+      </c>
+      <c r="C30">
+        <v>0.4</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>-0.2</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>1.03640719835925</v>
+      </c>
+      <c r="J30">
+        <v>2.3571322494390801E-2</v>
+      </c>
+      <c r="K30">
+        <v>0.63229862042353102</v>
+      </c>
+      <c r="L30">
+        <v>1.5054845524070799</v>
+      </c>
+      <c r="N30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>1.8</v>
+      </c>
+      <c r="C31">
+        <v>0.4</v>
+      </c>
+      <c r="D31">
+        <v>0.2</v>
+      </c>
+      <c r="E31">
+        <v>-0.2</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <v>0.95306140886294</v>
+      </c>
+      <c r="J31">
+        <v>2.1205413379844901E-2</v>
+      </c>
+      <c r="K31">
+        <v>0.605880387727873</v>
+      </c>
+      <c r="L31">
+        <v>1.37017314744728</v>
+      </c>
+      <c r="N31" t="s">
+        <v>32</v>
+      </c>
+      <c r="O31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>1.8</v>
+      </c>
+      <c r="C32">
+        <v>0.2</v>
+      </c>
+      <c r="D32">
+        <v>0.2</v>
+      </c>
+      <c r="E32">
+        <v>-0.2</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0.80400977272836904</v>
+      </c>
+      <c r="J32">
+        <v>1.6332356162736601E-2</v>
+      </c>
+      <c r="K32">
+        <v>0.743403569328692</v>
+      </c>
+      <c r="L32">
+        <v>1.1583203472585</v>
+      </c>
+      <c r="N32" t="s">
+        <v>33</v>
+      </c>
+      <c r="O32" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>1.8</v>
+      </c>
+      <c r="C33">
+        <v>0.1</v>
+      </c>
+      <c r="D33">
+        <v>0.2</v>
+      </c>
+      <c r="E33">
+        <v>-0.2</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0.733291384924316</v>
+      </c>
+      <c r="J33">
+        <v>1.4862617348011999E-2</v>
+      </c>
+      <c r="K33">
+        <v>0.90981751657461596</v>
+      </c>
+      <c r="L33">
+        <v>1.26131417500118</v>
+      </c>
+      <c r="N33" t="s">
+        <v>34</v>
+      </c>
+      <c r="O33" s="2"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>1.8</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0.2</v>
+      </c>
+      <c r="E34">
+        <v>-0.2</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>0.68328936545629204</v>
+      </c>
+      <c r="J34">
+        <v>1.3729679906534901E-2</v>
+      </c>
+      <c r="K34">
+        <v>1.50300265742582</v>
+      </c>
+      <c r="L34">
+        <v>1.2788913889436799</v>
+      </c>
+      <c r="N34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35">
+        <v>0.2</v>
+      </c>
+      <c r="D35">
+        <v>0.2</v>
+      </c>
+      <c r="E35">
+        <v>-0.2</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>0.74879183378748204</v>
+      </c>
+      <c r="J35">
+        <v>1.53985940271767E-2</v>
+      </c>
+      <c r="K35">
+        <v>0.67517334843716204</v>
+      </c>
+      <c r="L35">
+        <v>1.0994961524920699</v>
+      </c>
+      <c r="N35" t="s">
+        <v>36</v>
+      </c>
+      <c r="O35" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C36">
+        <v>0.2</v>
+      </c>
+      <c r="D36">
+        <v>0.2</v>
+      </c>
+      <c r="E36">
+        <v>-0.2</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>0.70125790297026602</v>
+      </c>
+      <c r="J36">
+        <v>1.45957825823845E-2</v>
+      </c>
+      <c r="K36">
+        <v>0.62285968245092704</v>
+      </c>
+      <c r="L36">
+        <v>1.0475824121584301</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>2.5</v>
+      </c>
+      <c r="C37">
+        <v>0.2</v>
+      </c>
+      <c r="D37">
+        <v>0.2</v>
+      </c>
+      <c r="E37">
+        <v>-0.2</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>0.64015631319982003</v>
+      </c>
+      <c r="J37">
+        <v>1.35801227661456E-2</v>
+      </c>
+      <c r="K37">
+        <v>0.55940221776199595</v>
+      </c>
+      <c r="L37">
+        <v>0.98551667603406201</v>
+      </c>
+      <c r="N37" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>3</v>
+      </c>
+      <c r="C38">
+        <v>0.2</v>
+      </c>
+      <c r="D38">
+        <v>0.2</v>
+      </c>
+      <c r="E38">
+        <v>-0.2</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>0.55768971075996498</v>
+      </c>
+      <c r="J38">
+        <v>1.22539695398521E-2</v>
+      </c>
+      <c r="K38">
+        <v>0.48194295856817299</v>
+      </c>
+      <c r="L38">
+        <v>0.90792969123067602</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>3.5</v>
+      </c>
+      <c r="C39">
+        <v>0.2</v>
+      </c>
+      <c r="D39">
+        <v>0.2</v>
+      </c>
+      <c r="E39">
+        <v>-0.2</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>0.492721293463945</v>
+      </c>
+      <c r="J39">
+        <v>1.12955301914836E-2</v>
+      </c>
+      <c r="K39">
+        <v>0.42272130458136697</v>
+      </c>
+      <c r="L39">
+        <v>0.85149056955977198</v>
+      </c>
+      <c r="N39" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>4</v>
+      </c>
+      <c r="C40">
+        <v>0.2</v>
+      </c>
+      <c r="D40">
+        <v>0.2</v>
+      </c>
+      <c r="E40">
+        <v>-0.2</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0.55064805182252197</v>
+      </c>
+      <c r="J40">
+        <v>0.75769029382077502</v>
+      </c>
+      <c r="K40">
+        <v>1.4121569642574401</v>
+      </c>
+      <c r="L40">
+        <v>1.6621444773856799</v>
+      </c>
+      <c r="N40" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41">
+        <v>3.2</v>
+      </c>
+      <c r="C41">
+        <v>0.2</v>
+      </c>
+      <c r="D41">
+        <v>0.2</v>
+      </c>
+      <c r="E41">
+        <v>-0.2</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>0.52995207695677304</v>
+      </c>
+      <c r="J41">
+        <v>1.18243224701363E-2</v>
+      </c>
+      <c r="K41">
+        <v>0.45908533568385701</v>
+      </c>
+      <c r="L41">
+        <v>0.88418467758623798</v>
+      </c>
+      <c r="N41" t="s">
+        <v>42</v>
+      </c>
+      <c r="O41" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43">
+        <v>3</v>
+      </c>
+      <c r="C43">
+        <v>0.2</v>
+      </c>
+      <c r="D43">
+        <v>0.2</v>
+      </c>
+      <c r="E43">
+        <v>-0.3</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>3.9737893848898298</v>
+      </c>
+      <c r="J43">
+        <v>3.5921314807397602</v>
+      </c>
+      <c r="K43">
+        <v>17.382264107070601</v>
+      </c>
+      <c r="L43">
+        <v>29.324448533950999</v>
+      </c>
+      <c r="N43" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>3</v>
+      </c>
+      <c r="C44">
+        <v>0.2</v>
+      </c>
+      <c r="D44">
+        <v>0.2</v>
+      </c>
+      <c r="E44">
+        <v>-0.1</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>0.80770380507239403</v>
+      </c>
+      <c r="J44">
+        <v>1.83855651020189E-2</v>
+      </c>
+      <c r="K44">
+        <v>0.573543422248741</v>
+      </c>
+      <c r="L44">
+        <v>1.4223608539275101</v>
+      </c>
+      <c r="N44" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="C45">
+        <v>0.2</v>
+      </c>
+      <c r="D45">
+        <v>0.2</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>2.4539198680805101</v>
+      </c>
+      <c r="J45">
+        <v>0.13211658134863499</v>
+      </c>
+      <c r="K45">
+        <v>1.0265463594289199</v>
+      </c>
+      <c r="L45">
+        <v>5.6198710475307898</v>
+      </c>
+      <c r="N45" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46">
+        <v>3</v>
+      </c>
+      <c r="C46">
+        <v>0.2</v>
+      </c>
+      <c r="D46">
+        <v>0.4</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>1.5193263771388399</v>
+      </c>
+      <c r="J46">
+        <v>4.78332457987862E-2</v>
+      </c>
+      <c r="K46">
+        <v>0.74546028015713195</v>
+      </c>
+      <c r="L46">
+        <v>4.2616158865210201</v>
+      </c>
+      <c r="N46" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47">
+        <v>3</v>
+      </c>
+      <c r="C47">
+        <v>0.2</v>
+      </c>
+      <c r="D47">
+        <v>0.6</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>1.0927626951384199</v>
+      </c>
+      <c r="J47">
+        <v>2.6473507520016901E-2</v>
+      </c>
+      <c r="K47">
+        <v>0.64358248937999296</v>
+      </c>
+      <c r="L47">
+        <v>2.4450320894137798</v>
+      </c>
+      <c r="N47" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>3</v>
+      </c>
+      <c r="C48">
+        <v>0.2</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>16.4130139895267</v>
+      </c>
+      <c r="J48">
+        <v>0.619219261399649</v>
+      </c>
+      <c r="K48">
+        <v>0.767820976828961</v>
+      </c>
+      <c r="L48">
+        <v>9.1220750444667704</v>
+      </c>
+      <c r="N48" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49">
+        <v>3</v>
+      </c>
+      <c r="C49">
+        <v>0.2</v>
+      </c>
+      <c r="D49">
+        <v>0.8</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <v>0.74449461717052201</v>
+      </c>
+      <c r="J49">
+        <v>0.36297675737641999</v>
+      </c>
+      <c r="K49">
+        <v>0.56482530064813496</v>
+      </c>
+      <c r="L49">
+        <v>1.72250188305564</v>
+      </c>
+      <c r="N49" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51">
+        <v>3</v>
+      </c>
+      <c r="C51">
+        <v>0.2</v>
+      </c>
+      <c r="D51">
+        <v>0.3</v>
+      </c>
+      <c r="E51">
+        <v>-0.2</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <v>1.1758926996574299</v>
+      </c>
+      <c r="J51">
+        <v>1.41380731684507</v>
+      </c>
+      <c r="K51">
+        <v>1.25646115108854</v>
+      </c>
+      <c r="L51">
+        <v>2.0824282506694098</v>
+      </c>
+      <c r="N51" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>3</v>
+      </c>
+      <c r="C52">
+        <v>0.2</v>
+      </c>
+      <c r="D52">
+        <v>0.1</v>
+      </c>
+      <c r="E52">
+        <v>-0.2</v>
+      </c>
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="I52">
+        <v>0.58084195986799503</v>
+      </c>
+      <c r="J52">
+        <v>1.28101379563615E-2</v>
+      </c>
+      <c r="K52">
+        <v>0.49012735875930002</v>
+      </c>
+      <c r="L52">
+        <v>0.94896815618400399</v>
+      </c>
+      <c r="N52" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>56</v>
+      </c>
+      <c r="B53">
+        <v>3</v>
+      </c>
+      <c r="C53">
+        <v>0.2</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>-0.2</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="I53">
+        <v>0.60704569239098505</v>
+      </c>
+      <c r="J53">
+        <v>1.3468628817882401E-2</v>
+      </c>
+      <c r="K53">
+        <v>0.50043854750763095</v>
+      </c>
+      <c r="L53">
+        <v>0.99494854744850902</v>
+      </c>
+      <c r="N53" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>58</v>
+      </c>
+      <c r="B54">
+        <v>3</v>
+      </c>
+      <c r="C54">
+        <v>0.2</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>-0.25</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="I54">
+        <v>0.52765884296688903</v>
+      </c>
+      <c r="J54">
+        <v>1.17355143368887E-2</v>
+      </c>
+      <c r="K54">
+        <v>0.47188088356695801</v>
+      </c>
+      <c r="L54">
+        <v>0.85921890761032804</v>
+      </c>
+      <c r="N54" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <v>3</v>
+      </c>
+      <c r="C55">
+        <v>0.2</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>-0.3</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="I55">
+        <v>0.45926505025900299</v>
+      </c>
+      <c r="J55">
+        <v>1.07907535135291E-2</v>
+      </c>
+      <c r="K55">
+        <v>0.47564988860850199</v>
+      </c>
+      <c r="L55">
+        <v>0.76971399098628601</v>
+      </c>
+      <c r="N55" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <v>3</v>
+      </c>
+      <c r="C56">
+        <v>0.2</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>-0.28000000000000003</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <v>0.48920230581558</v>
+      </c>
+      <c r="J56">
+        <v>1.10206296578436E-2</v>
+      </c>
+      <c r="K56">
+        <v>0.46416492420864802</v>
+      </c>
+      <c r="L56">
+        <v>0.80288481097966302</v>
+      </c>
+      <c r="N56" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New gains, added offset possibilities in sim
</commit_message>
<xml_diff>
--- a/Gainsheet.xlsx
+++ b/Gainsheet.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hampu\Documents\Atmel Studio\7.0\AutoBike-Simulation-MDH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{189BF987-1A11-4B59-8560-AD1DD4641DB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F47458-EE0B-45F0-836E-E3F6B80B1EBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="82">
   <si>
     <t>I Lat</t>
   </si>
@@ -212,14 +213,85 @@
   </si>
   <si>
     <t>Not as good again</t>
+  </si>
+  <si>
+    <t>Ocsillations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good </t>
+  </si>
+  <si>
+    <t>Gå igenom igen</t>
+  </si>
+  <si>
+    <t>Removing integration</t>
+  </si>
+  <si>
+    <t>Best for non heading</t>
+  </si>
+  <si>
+    <t>Crash</t>
+  </si>
+  <si>
+    <t>How high can P go?</t>
+  </si>
+  <si>
+    <t>How fucking high is possible?</t>
+  </si>
+  <si>
+    <t>Okey that is to much</t>
+  </si>
+  <si>
+    <t>Seem to be able to scale just lateral gain</t>
+  </si>
+  <si>
+    <t>Best</t>
+  </si>
+  <si>
+    <t>0.25 phead is unstable</t>
+  </si>
+  <si>
+    <t>unstable</t>
+  </si>
+  <si>
+    <t>not better</t>
+  </si>
+  <si>
+    <t>Integration on heading</t>
+  </si>
+  <si>
+    <t>Ocsillation in rrt</t>
+  </si>
+  <si>
+    <t>Init 40d yaw</t>
+  </si>
+  <si>
+    <t>5m y added</t>
+  </si>
+  <si>
+    <t>10m y is to much</t>
+  </si>
+  <si>
+    <t>Nice piruett at 10m but finds goal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -247,12 +319,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -535,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2385,4 +2460,2551 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B706E9A-D8F2-483B-90DB-055EAB945C48}">
+  <dimension ref="A1:AE71"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="4" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" style="3" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" customWidth="1"/>
+    <col min="15" max="15" width="13.85546875" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" customWidth="1"/>
+    <col min="18" max="18" width="13.7109375" style="3" customWidth="1"/>
+    <col min="19" max="19" width="11.28515625" style="3" customWidth="1"/>
+    <col min="20" max="20" width="12.140625" style="3" customWidth="1"/>
+    <col min="21" max="21" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>0.6</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <v>3.9578960829832299</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.107882851581642</v>
+      </c>
+      <c r="K2" s="3">
+        <v>4.1765720444503103</v>
+      </c>
+      <c r="L2" s="3">
+        <v>4.5827672298253201</v>
+      </c>
+    </row>
+    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>0.2</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
+        <v>6.7491484634246799</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0.18896926000321701</v>
+      </c>
+      <c r="K3" s="3">
+        <v>10.2870279698696</v>
+      </c>
+      <c r="L3" s="3">
+        <v>10.1752406373755</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>0.8</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3">
+        <v>3.2006817268871699</v>
+      </c>
+      <c r="J4" s="3">
+        <v>8.9841311492131495E-2</v>
+      </c>
+      <c r="K4" s="3">
+        <v>3.44514032352243</v>
+      </c>
+      <c r="L4" s="3">
+        <v>4.9302833782958801</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>2.73416854737716</v>
+      </c>
+      <c r="J5" s="3">
+        <v>8.1259924108962406E-2</v>
+      </c>
+      <c r="K5" s="3">
+        <v>2.9351558547239001</v>
+      </c>
+      <c r="L5" s="3">
+        <v>4.3190580136484904</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0.1</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3">
+        <v>2.5616039024652202</v>
+      </c>
+      <c r="J6" s="3">
+        <v>7.0949899568876498E-2</v>
+      </c>
+      <c r="K6" s="3">
+        <v>2.8481232951683402</v>
+      </c>
+      <c r="L6" s="3">
+        <v>3.80717129240031</v>
+      </c>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0.5</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
+        <v>2.0723682020398799</v>
+      </c>
+      <c r="J7" s="3">
+        <v>4.7564024255351098E-2</v>
+      </c>
+      <c r="K7" s="3">
+        <v>2.6372897229311798</v>
+      </c>
+      <c r="L7" s="3">
+        <v>2.9758687774537198</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3">
+        <v>1.68381425165431</v>
+      </c>
+      <c r="J8" s="3">
+        <v>3.5440566711753101E-2</v>
+      </c>
+      <c r="K8" s="3">
+        <v>2.5184141255276802</v>
+      </c>
+      <c r="L8" s="3">
+        <v>2.4687303575685702</v>
+      </c>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>0.5</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3">
+        <v>3.1001862339975599</v>
+      </c>
+      <c r="J9" s="3">
+        <v>6.8581290280160495E-2</v>
+      </c>
+      <c r="K9" s="3">
+        <v>4.5885171237449001</v>
+      </c>
+      <c r="L9" s="3">
+        <v>4.1289435811361299</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0.81649027710562505</v>
+      </c>
+      <c r="J10" s="3">
+        <v>1.80841465584398E-2</v>
+      </c>
+      <c r="K10" s="3">
+        <v>1.2996332612128001</v>
+      </c>
+      <c r="L10" s="3">
+        <v>1.3880064546778501</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0.5</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3">
+        <v>1.06942870229112</v>
+      </c>
+      <c r="J11" s="3">
+        <v>2.4721592956352501E-2</v>
+      </c>
+      <c r="K11" s="3">
+        <v>1.3525193962469899</v>
+      </c>
+      <c r="L11" s="3">
+        <v>1.6783664964423399</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>1.5</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0.63001787803351605</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0.23611526621657</v>
+      </c>
+      <c r="K12" s="3">
+        <v>1.1362969381140799</v>
+      </c>
+      <c r="L12" s="3">
+        <v>1.0625431509257199</v>
+      </c>
+      <c r="M12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="I13" s="3">
+        <v>0.48915733409353102</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0.166811330164543</v>
+      </c>
+      <c r="K13" s="3">
+        <v>1.7676467575187</v>
+      </c>
+      <c r="L13" s="3">
+        <v>1.2408476990355899</v>
+      </c>
+      <c r="M13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>2.5</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="I14" s="3">
+        <v>0.63726554114502298</v>
+      </c>
+      <c r="J14" s="3">
+        <v>1.46068694477991E-2</v>
+      </c>
+      <c r="K14" s="3">
+        <v>1.0431894507142001</v>
+      </c>
+      <c r="L14" s="3">
+        <v>1.1658602655071899</v>
+      </c>
+      <c r="M14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>2.5</v>
+      </c>
+      <c r="C15">
+        <v>0.1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="I15" s="3">
+        <v>0.70347077832068905</v>
+      </c>
+      <c r="J15" s="3">
+        <v>1.6446953703349199E-2</v>
+      </c>
+      <c r="K15" s="3">
+        <v>0.65935918355249901</v>
+      </c>
+      <c r="L15" s="3">
+        <v>1.22487681335564</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>2.5</v>
+      </c>
+      <c r="C16">
+        <v>0.2</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="I16" s="3">
+        <v>0.80175735468855902</v>
+      </c>
+      <c r="J16" s="3">
+        <v>1.92171158465489E-2</v>
+      </c>
+      <c r="K16" s="3">
+        <v>0.58728640295893497</v>
+      </c>
+      <c r="L16" s="3">
+        <v>1.3465662182988001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>0.2</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="I17" s="3">
+        <v>0.580335697845481</v>
+      </c>
+      <c r="J17" s="3">
+        <v>0.174636903020498</v>
+      </c>
+      <c r="K17" s="3">
+        <v>0.47698945492885902</v>
+      </c>
+      <c r="L17" s="3">
+        <v>1.3918358349095801</v>
+      </c>
+      <c r="M17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>2.8</v>
+      </c>
+      <c r="C18">
+        <v>0.2</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="I18" s="3">
+        <v>0.68009274236510797</v>
+      </c>
+      <c r="J18" s="3">
+        <v>1.6590333004832401E-2</v>
+      </c>
+      <c r="K18" s="3">
+        <v>0.51343981325775001</v>
+      </c>
+      <c r="L18" s="3">
+        <v>1.2236838006445401</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>2.8</v>
+      </c>
+      <c r="C19">
+        <v>0.2</v>
+      </c>
+      <c r="D19">
+        <v>1.2</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="I19" s="3">
+        <v>2.6587897673539098</v>
+      </c>
+      <c r="J19" s="3">
+        <v>0.34015553939472298</v>
+      </c>
+      <c r="K19" s="3">
+        <v>1.61709960723375</v>
+      </c>
+      <c r="L19" s="3">
+        <v>8.6217658027527104</v>
+      </c>
+      <c r="M19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>2.8</v>
+      </c>
+      <c r="C20">
+        <v>0.1</v>
+      </c>
+      <c r="D20">
+        <v>1.2</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="I20" s="3">
+        <v>0.38666780592315397</v>
+      </c>
+      <c r="J20" s="3">
+        <v>1.9315960862102901</v>
+      </c>
+      <c r="K20" s="3">
+        <v>0.54592314602793601</v>
+      </c>
+      <c r="L20" s="3">
+        <v>0.83537596263740999</v>
+      </c>
+      <c r="M20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>2.8</v>
+      </c>
+      <c r="C21">
+        <v>0.3</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="I21" s="3">
+        <v>0.77910385893466105</v>
+      </c>
+      <c r="J21" s="3">
+        <v>1.97666541757557E-2</v>
+      </c>
+      <c r="K21" s="3">
+        <v>0.49674831657950103</v>
+      </c>
+      <c r="L21" s="3">
+        <v>1.5330761061242899</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>0.3</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="I22" s="3">
+        <v>0.67226837918541504</v>
+      </c>
+      <c r="J22" s="3">
+        <v>0.71821443980982502</v>
+      </c>
+      <c r="K22" s="3">
+        <v>0.46592450462541801</v>
+      </c>
+      <c r="L22" s="3">
+        <v>1.7270939640873699</v>
+      </c>
+      <c r="M22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23">
+        <v>2.8</v>
+      </c>
+      <c r="C23">
+        <v>0.1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="I23" s="3">
+        <v>0.60742506581530498</v>
+      </c>
+      <c r="J23" s="3">
+        <v>1.45746402773005E-2</v>
+      </c>
+      <c r="K23" s="3">
+        <v>0.58773996812187101</v>
+      </c>
+      <c r="L23" s="3">
+        <v>1.1115374190314899</v>
+      </c>
+      <c r="M23" t="s">
+        <v>66</v>
+      </c>
+      <c r="R23" s="3">
+        <v>0.86001500996563496</v>
+      </c>
+      <c r="S23" s="3">
+        <v>0.50100554470358905</v>
+      </c>
+      <c r="T23" s="3">
+        <v>0.97232700760367796</v>
+      </c>
+      <c r="U23" s="3">
+        <v>1.1642512996067</v>
+      </c>
+      <c r="W23" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y23" s="5">
+        <v>2.26901864123771</v>
+      </c>
+      <c r="Z23">
+        <v>1.85005294540319</v>
+      </c>
+      <c r="AA23">
+        <v>2.2475403669895</v>
+      </c>
+      <c r="AB23">
+        <v>1.7822612122985899</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>2.8</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="I24" s="3">
+        <v>0.55893808009300106</v>
+      </c>
+      <c r="J24" s="3">
+        <v>1.3153422739757999E-2</v>
+      </c>
+      <c r="K24" s="3">
+        <v>0.93348630534459698</v>
+      </c>
+      <c r="L24" s="3">
+        <v>1.0560991687771699</v>
+      </c>
+      <c r="W24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>2.9</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="I25" s="3">
+        <v>0.53763674731106703</v>
+      </c>
+      <c r="J25" s="3">
+        <v>5.6116852544799603E-2</v>
+      </c>
+      <c r="K25" s="3">
+        <v>0.89187868448542595</v>
+      </c>
+      <c r="L25" s="3">
+        <v>1.0224350484245699</v>
+      </c>
+      <c r="M25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>2.8</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="I26" s="3">
+        <v>0.47521722135894701</v>
+      </c>
+      <c r="J26" s="3">
+        <v>0.27144887505818199</v>
+      </c>
+      <c r="K26" s="3">
+        <v>0.77025358095160001</v>
+      </c>
+      <c r="L26" s="3">
+        <v>1.3878672749165</v>
+      </c>
+      <c r="M26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0.5</v>
+      </c>
+      <c r="E30">
+        <v>-0.1</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="I30" s="3">
+        <v>1.12523034693642</v>
+      </c>
+      <c r="J30" s="3">
+        <v>2.3451199996074298E-2</v>
+      </c>
+      <c r="K30" s="3">
+        <v>2.3619094835435002</v>
+      </c>
+      <c r="L30" s="3">
+        <v>1.9661299641662899</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0.5</v>
+      </c>
+      <c r="E31">
+        <v>-0.2</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="I31" s="3">
+        <v>0.82450322985236801</v>
+      </c>
+      <c r="J31" s="3">
+        <v>7.2053149734578703</v>
+      </c>
+      <c r="K31" s="3">
+        <v>4.1922818914723097</v>
+      </c>
+      <c r="L31" s="3">
+        <v>7.2680937914476802</v>
+      </c>
+      <c r="M31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>1.3</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0.5</v>
+      </c>
+      <c r="E32">
+        <v>-0.1</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="I32" s="3">
+        <v>0.93917597259642505</v>
+      </c>
+      <c r="J32" s="3">
+        <v>2.00126877354471E-2</v>
+      </c>
+      <c r="K32" s="3">
+        <v>1.8794976711498601</v>
+      </c>
+      <c r="L32" s="3">
+        <v>1.6281527186840301</v>
+      </c>
+    </row>
+    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>1.3</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>-0.1</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="I33" s="3">
+        <v>1.06007623718849</v>
+      </c>
+      <c r="J33" s="3">
+        <v>2.2827444232747299E-2</v>
+      </c>
+      <c r="K33" s="3">
+        <v>1.9161760997041299</v>
+      </c>
+      <c r="L33" s="3">
+        <v>1.7406095828621999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>1.3</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>-0.2</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="I34" s="3">
+        <v>0.76346182132401597</v>
+      </c>
+      <c r="J34" s="3">
+        <v>1.6790319980550701E-2</v>
+      </c>
+      <c r="K34" s="3">
+        <v>1.8098077782695201</v>
+      </c>
+      <c r="L34" s="3">
+        <v>1.4571406587179601</v>
+      </c>
+    </row>
+    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>1.3</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>-0.2</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0.1</v>
+      </c>
+      <c r="I35" s="3">
+        <v>19.637410644569599</v>
+      </c>
+      <c r="J35" s="3">
+        <v>6.1060917688305798</v>
+      </c>
+      <c r="K35" s="3">
+        <v>17.875412690307598</v>
+      </c>
+      <c r="L35" s="3">
+        <v>71.991688931682006</v>
+      </c>
+      <c r="M35" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>1.3</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>-0.2</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0.02</v>
+      </c>
+      <c r="I36" s="3">
+        <v>21.726131791840299</v>
+      </c>
+      <c r="J36" s="3">
+        <v>21.171933986402198</v>
+      </c>
+      <c r="K36" s="3">
+        <v>24.803254985280699</v>
+      </c>
+      <c r="L36" s="3">
+        <v>20.7393839337137</v>
+      </c>
+    </row>
+    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>1.3</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>-0.2</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="I37" s="3">
+        <v>1.5211735194951701</v>
+      </c>
+      <c r="J37" s="3">
+        <v>9.3578048997234403E-2</v>
+      </c>
+      <c r="K37" s="3">
+        <v>0.97438015201005301</v>
+      </c>
+      <c r="L37" s="3">
+        <v>15.8089742099997</v>
+      </c>
+      <c r="M37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>1.3</v>
+      </c>
+      <c r="C38">
+        <v>0.5</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>-0.2</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="I38" s="3">
+        <v>1.0888404976245101</v>
+      </c>
+      <c r="J38" s="3">
+        <v>2.9892141127546901E-2</v>
+      </c>
+      <c r="K38" s="3">
+        <v>0.66752801020931196</v>
+      </c>
+      <c r="L38" s="3">
+        <v>1.635588809985</v>
+      </c>
+    </row>
+    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>1.3</v>
+      </c>
+      <c r="C39">
+        <v>0.2</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>-0.2</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="I39" s="3">
+        <v>0.89493368344406898</v>
+      </c>
+      <c r="J39" s="3">
+        <v>1.9888204397979101E-2</v>
+      </c>
+      <c r="K39" s="3">
+        <v>0.89939686131306296</v>
+      </c>
+      <c r="L39" s="3">
+        <v>1.2712843799728799</v>
+      </c>
+    </row>
+    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>1.3</v>
+      </c>
+      <c r="C40">
+        <v>0.1</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>-0.2</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="I40" s="3">
+        <v>0.805918773061847</v>
+      </c>
+      <c r="J40" s="3">
+        <v>1.8144303345966801E-2</v>
+      </c>
+      <c r="K40" s="3">
+        <v>1.0987943346751701</v>
+      </c>
+      <c r="L40" s="3">
+        <v>1.4595529663047999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>1.6</v>
+      </c>
+      <c r="C41">
+        <v>0.1</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>-0.2</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="I41" s="3">
+        <v>0.725801652714963</v>
+      </c>
+      <c r="J41" s="3">
+        <v>1.6370418177744699E-2</v>
+      </c>
+      <c r="K41" s="3">
+        <v>0.91503663634616506</v>
+      </c>
+      <c r="L41" s="3">
+        <v>1.2543077863719401</v>
+      </c>
+      <c r="AB41" s="3"/>
+      <c r="AC41" s="3"/>
+      <c r="AD41" s="3"/>
+      <c r="AE41" s="3"/>
+    </row>
+    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>1.8</v>
+      </c>
+      <c r="C42">
+        <v>0.1</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>-0.2</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="I42" s="3">
+        <v>0.67717597653497996</v>
+      </c>
+      <c r="J42" s="3">
+        <v>1.54471542770042E-2</v>
+      </c>
+      <c r="K42" s="3">
+        <v>0.82379715850880797</v>
+      </c>
+      <c r="L42" s="3">
+        <v>1.1616886927827501</v>
+      </c>
+      <c r="AB42" s="3"/>
+      <c r="AC42" s="3"/>
+      <c r="AD42" s="3"/>
+      <c r="AE42" s="3"/>
+    </row>
+    <row r="43" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43">
+        <v>2.5</v>
+      </c>
+      <c r="C43">
+        <v>0.1</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>-0.2</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="I43" s="3">
+        <v>0.54796788392650297</v>
+      </c>
+      <c r="J43" s="3">
+        <v>1.3162984208949499E-2</v>
+      </c>
+      <c r="K43" s="3">
+        <v>0.61708609351967603</v>
+      </c>
+      <c r="L43" s="3">
+        <v>0.957331390244891</v>
+      </c>
+      <c r="AB43" s="3"/>
+      <c r="AC43" s="3"/>
+      <c r="AD43" s="3"/>
+      <c r="AE43" s="3"/>
+    </row>
+    <row r="44" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>3</v>
+      </c>
+      <c r="C44">
+        <v>0.1</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>-0.2</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="I44" s="3">
+        <v>0.484286963089468</v>
+      </c>
+      <c r="J44" s="3">
+        <v>1.20669271855056E-2</v>
+      </c>
+      <c r="K44" s="3">
+        <v>0.52743638519027003</v>
+      </c>
+      <c r="L44" s="3">
+        <v>0.87265407537519701</v>
+      </c>
+      <c r="R44" s="3">
+        <v>0.56614948617347105</v>
+      </c>
+      <c r="S44" s="3">
+        <v>0.29286574718351799</v>
+      </c>
+      <c r="T44" s="3">
+        <v>0.72838711420015201</v>
+      </c>
+      <c r="U44" s="3">
+        <v>0.90109246346467498</v>
+      </c>
+      <c r="Y44">
+        <v>1.74985779736085</v>
+      </c>
+      <c r="Z44">
+        <v>1.4219488931339099</v>
+      </c>
+      <c r="AA44">
+        <v>1.8537441763315201</v>
+      </c>
+      <c r="AB44" s="3">
+        <v>1.4254613624174499</v>
+      </c>
+      <c r="AC44" s="3"/>
+      <c r="AD44" s="3"/>
+      <c r="AE44" s="3"/>
+    </row>
+    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>3.5</v>
+      </c>
+      <c r="C45">
+        <v>0.1</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>-0.2</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="I45" s="3">
+        <v>0.43167918939102101</v>
+      </c>
+      <c r="J45" s="3">
+        <v>1.12299458887538E-2</v>
+      </c>
+      <c r="K45" s="3">
+        <v>0.46143158466152601</v>
+      </c>
+      <c r="L45" s="3">
+        <v>0.81074412478856805</v>
+      </c>
+      <c r="AB45" s="3"/>
+      <c r="AC45" s="3"/>
+      <c r="AD45" s="3"/>
+      <c r="AE45" s="3"/>
+    </row>
+    <row r="46" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>4</v>
+      </c>
+      <c r="C46">
+        <v>0.1</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>-0.2</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="I46" s="3">
+        <v>0.39132233077754802</v>
+      </c>
+      <c r="J46" s="3">
+        <v>1.0569511933062801E-2</v>
+      </c>
+      <c r="K46" s="3">
+        <v>0.41234910918992701</v>
+      </c>
+      <c r="L46" s="3">
+        <v>0.758594623376729</v>
+      </c>
+      <c r="AB46" s="3"/>
+      <c r="AC46" s="3"/>
+      <c r="AD46" s="3"/>
+      <c r="AE46" s="3"/>
+    </row>
+    <row r="47" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>4.5</v>
+      </c>
+      <c r="C47">
+        <v>0.1</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>-0.2</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="I47" s="3">
+        <v>0.357823300450406</v>
+      </c>
+      <c r="J47" s="3">
+        <v>1.00363218859248E-2</v>
+      </c>
+      <c r="K47" s="3">
+        <v>0.37122546891713398</v>
+      </c>
+      <c r="L47" s="3">
+        <v>0.70961993512028199</v>
+      </c>
+      <c r="AB47" s="3"/>
+      <c r="AC47" s="3"/>
+      <c r="AD47" s="3"/>
+      <c r="AE47" s="3"/>
+    </row>
+    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B48">
+        <v>5</v>
+      </c>
+      <c r="C48">
+        <v>0.1</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>-0.2</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="I48" s="3">
+        <v>0.329384825114515</v>
+      </c>
+      <c r="J48" s="3">
+        <v>9.5990131825856098E-3</v>
+      </c>
+      <c r="K48" s="3">
+        <v>0.33984160422110399</v>
+      </c>
+      <c r="L48" s="3">
+        <v>0.66260532738514499</v>
+      </c>
+      <c r="R48" s="3">
+        <v>0.40431964520664598</v>
+      </c>
+      <c r="S48" s="3">
+        <v>0.20618648853508401</v>
+      </c>
+      <c r="T48" s="3">
+        <v>0.45045824717681998</v>
+      </c>
+      <c r="U48" s="3">
+        <v>0.67083082677276396</v>
+      </c>
+      <c r="Y48">
+        <v>2.2719161275492499</v>
+      </c>
+      <c r="Z48">
+        <v>1.9212413168214899</v>
+      </c>
+      <c r="AA48">
+        <v>2.3048741010160398</v>
+      </c>
+      <c r="AB48" s="3">
+        <v>1.66704290845173</v>
+      </c>
+      <c r="AC48" s="3"/>
+      <c r="AD48" s="3"/>
+      <c r="AE48" s="3"/>
+    </row>
+    <row r="49" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B49">
+        <v>5</v>
+      </c>
+      <c r="C49">
+        <v>0.2</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>-0.2</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="I49" s="3">
+        <v>0.348381608218156</v>
+      </c>
+      <c r="J49" s="3">
+        <v>1.03656682423656E-2</v>
+      </c>
+      <c r="K49" s="3">
+        <v>0.29149859513716397</v>
+      </c>
+      <c r="L49" s="3">
+        <v>0.69841633006716597</v>
+      </c>
+      <c r="W49" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB49" s="3"/>
+      <c r="AC49" s="3"/>
+      <c r="AD49" s="3"/>
+      <c r="AE49" s="3"/>
+    </row>
+    <row r="50" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>5</v>
+      </c>
+      <c r="C50">
+        <v>0.3</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>-0.2</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="I50" s="3">
+        <v>0.37244401075015798</v>
+      </c>
+      <c r="J50" s="3">
+        <v>1.13556629498178E-2</v>
+      </c>
+      <c r="K50" s="3">
+        <v>0.26761419596657399</v>
+      </c>
+      <c r="L50" s="3">
+        <v>0.767984023491877</v>
+      </c>
+      <c r="AB50" s="3"/>
+      <c r="AC50" s="3"/>
+      <c r="AD50" s="3"/>
+      <c r="AE50" s="3"/>
+    </row>
+    <row r="51" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>5</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>-0.2</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="I51" s="3">
+        <v>0.31578272876569402</v>
+      </c>
+      <c r="J51" s="3">
+        <v>8.9831600103302493E-3</v>
+      </c>
+      <c r="K51" s="3">
+        <v>0.53142413166492197</v>
+      </c>
+      <c r="L51" s="3">
+        <v>0.64124604624616</v>
+      </c>
+      <c r="AB51" s="3"/>
+      <c r="AC51" s="3"/>
+      <c r="AD51" s="3"/>
+      <c r="AE51" s="3"/>
+    </row>
+    <row r="52" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>5</v>
+      </c>
+      <c r="C52">
+        <v>0.1</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>-0.1</v>
+      </c>
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="I52" s="3">
+        <v>0.452554311174788</v>
+      </c>
+      <c r="J52" s="3">
+        <v>1.3913618778343099E-2</v>
+      </c>
+      <c r="K52" s="3">
+        <v>0.380922335757789</v>
+      </c>
+      <c r="L52" s="3">
+        <v>0.90595621374656099</v>
+      </c>
+      <c r="AB52" s="3"/>
+      <c r="AC52" s="3"/>
+      <c r="AD52" s="3"/>
+      <c r="AE52" s="3"/>
+    </row>
+    <row r="53" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <v>5</v>
+      </c>
+      <c r="C53">
+        <v>0.1</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>-0.3</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="I53" s="3">
+        <v>15.308515303306701</v>
+      </c>
+      <c r="J53" s="3">
+        <v>16.113342116216302</v>
+      </c>
+      <c r="K53" s="3">
+        <v>15.3568272406799</v>
+      </c>
+      <c r="L53" s="3">
+        <v>47.882617777061398</v>
+      </c>
+      <c r="M53" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB53" s="3"/>
+      <c r="AC53" s="3"/>
+      <c r="AD53" s="3"/>
+      <c r="AE53" s="3"/>
+    </row>
+    <row r="54" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>69</v>
+      </c>
+      <c r="B54">
+        <v>6</v>
+      </c>
+      <c r="C54">
+        <v>0.1</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>-0.2</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="I54" s="3">
+        <v>0.28337665395925998</v>
+      </c>
+      <c r="J54" s="3">
+        <v>8.9354263821887804E-3</v>
+      </c>
+      <c r="K54" s="3">
+        <v>0.28802588223277797</v>
+      </c>
+      <c r="L54" s="3">
+        <v>0.57798695693366797</v>
+      </c>
+      <c r="AB54" s="3"/>
+      <c r="AC54" s="3"/>
+      <c r="AD54" s="3"/>
+      <c r="AE54" s="3"/>
+    </row>
+    <row r="55" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <v>7</v>
+      </c>
+      <c r="C55">
+        <v>0.1</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>-0.2</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="I55" s="3">
+        <v>0.247878797382136</v>
+      </c>
+      <c r="J55" s="3">
+        <v>8.4818724019189093E-3</v>
+      </c>
+      <c r="K55" s="3">
+        <v>0.24941883845636501</v>
+      </c>
+      <c r="L55" s="3">
+        <v>0.50673933963169604</v>
+      </c>
+      <c r="AB55" s="3"/>
+      <c r="AC55" s="3"/>
+      <c r="AD55" s="3"/>
+      <c r="AE55" s="3"/>
+    </row>
+    <row r="56" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B56">
+        <v>10</v>
+      </c>
+      <c r="C56">
+        <v>0.1</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>-0.2</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="I56" s="3">
+        <v>0.16973079894239801</v>
+      </c>
+      <c r="J56" s="3">
+        <v>0.72004663258048796</v>
+      </c>
+      <c r="K56" s="3">
+        <v>12.830625635570399</v>
+      </c>
+      <c r="L56" s="3">
+        <v>27.770822615376002</v>
+      </c>
+      <c r="M56" t="s">
+        <v>67</v>
+      </c>
+      <c r="N56" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB56" s="3"/>
+      <c r="AC56" s="3"/>
+      <c r="AD56" s="3"/>
+      <c r="AE56" s="3"/>
+    </row>
+    <row r="57" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B57">
+        <v>8</v>
+      </c>
+      <c r="C57">
+        <v>0.1</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>-0.2</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="I57" s="3">
+        <v>0.21840209888231499</v>
+      </c>
+      <c r="J57" s="3">
+        <v>8.2202306299579107E-3</v>
+      </c>
+      <c r="K57" s="3">
+        <v>0.220022802595636</v>
+      </c>
+      <c r="L57" s="3">
+        <v>0.44840632286107002</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB57" s="3"/>
+      <c r="AC57" s="3"/>
+      <c r="AD57" s="3"/>
+      <c r="AE57" s="3"/>
+    </row>
+    <row r="58" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B58">
+        <v>9</v>
+      </c>
+      <c r="C58">
+        <v>0.1</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>-0.2</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="I58" s="3">
+        <v>0.193090069786437</v>
+      </c>
+      <c r="J58" s="3">
+        <v>8.4438185276726196E-3</v>
+      </c>
+      <c r="K58" s="3">
+        <v>0.194558923009473</v>
+      </c>
+      <c r="L58" s="3">
+        <v>42.877004289064303</v>
+      </c>
+      <c r="M58" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB58" s="3"/>
+      <c r="AC58" s="3"/>
+      <c r="AD58" s="3"/>
+      <c r="AE58" s="3"/>
+    </row>
+    <row r="59" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B59">
+        <v>8.5</v>
+      </c>
+      <c r="C59">
+        <v>0.1</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>-0.2</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+      <c r="I59" s="3">
+        <v>0.20531231897257701</v>
+      </c>
+      <c r="J59" s="3">
+        <v>8.2103376639326795E-3</v>
+      </c>
+      <c r="K59" s="3">
+        <v>0.20613832476131999</v>
+      </c>
+      <c r="L59" s="3">
+        <v>0.42158025194620702</v>
+      </c>
+      <c r="M59" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB59" s="3"/>
+      <c r="AC59" s="3"/>
+      <c r="AD59" s="3"/>
+      <c r="AE59" s="3"/>
+    </row>
+    <row r="60" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B60">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="C60">
+        <v>0.1</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>-0.2</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="I60" s="3">
+        <v>0.19788991614684101</v>
+      </c>
+      <c r="J60" s="3">
+        <v>8.2918695558750095E-3</v>
+      </c>
+      <c r="K60" s="3">
+        <v>0.19913233611959399</v>
+      </c>
+      <c r="L60" s="3">
+        <v>0.40535708876434501</v>
+      </c>
+      <c r="N60" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB60" s="3"/>
+      <c r="AC60" s="3"/>
+      <c r="AD60" s="3"/>
+      <c r="AE60" s="3"/>
+    </row>
+    <row r="61" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B61">
+        <v>8.9</v>
+      </c>
+      <c r="C61">
+        <v>0.1</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>-0.2</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="I61" s="3">
+        <v>0.19547645074810199</v>
+      </c>
+      <c r="J61" s="3">
+        <v>8.3551382640506197E-3</v>
+      </c>
+      <c r="K61" s="3">
+        <v>0.19673082710140799</v>
+      </c>
+      <c r="L61" s="3">
+        <v>0.39266440377241602</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB61" s="3"/>
+      <c r="AC61" s="3"/>
+      <c r="AD61" s="3"/>
+      <c r="AE61" s="3"/>
+    </row>
+    <row r="62" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B62">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="C62">
+        <v>0.1</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>-0.15</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+      <c r="I62" s="3">
+        <v>0.217646255171216</v>
+      </c>
+      <c r="J62" s="3">
+        <v>9.2268067433461508E-3</v>
+      </c>
+      <c r="K62" s="3">
+        <v>0.209649118587137</v>
+      </c>
+      <c r="L62" s="3">
+        <v>0.44740215370637199</v>
+      </c>
+      <c r="M62" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB62" s="3"/>
+      <c r="AC62" s="3"/>
+      <c r="AD62" s="3"/>
+      <c r="AE62" s="3"/>
+    </row>
+    <row r="63" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B63">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="C63">
+        <v>0.1</v>
+      </c>
+      <c r="D63">
+        <v>0.05</v>
+      </c>
+      <c r="E63">
+        <v>-0.2</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="I63" s="3">
+        <v>4.6638026290516903</v>
+      </c>
+      <c r="J63" s="3">
+        <v>6.06937780118544</v>
+      </c>
+      <c r="K63" s="3">
+        <v>10.8314863409102</v>
+      </c>
+      <c r="L63" s="3">
+        <v>6.7123885481414201</v>
+      </c>
+      <c r="M63" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB63" s="3"/>
+      <c r="AC63" s="3"/>
+      <c r="AD63" s="3"/>
+      <c r="AE63" s="3"/>
+    </row>
+    <row r="64" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B64">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="C64">
+        <v>0.1</v>
+      </c>
+      <c r="D64">
+        <v>-0.05</v>
+      </c>
+      <c r="E64">
+        <v>-0.2</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+      <c r="I64" s="3">
+        <v>0.20650916723489801</v>
+      </c>
+      <c r="J64" s="3">
+        <v>8.4180547425808192E-3</v>
+      </c>
+      <c r="K64" s="3">
+        <v>0.204775763364448</v>
+      </c>
+      <c r="L64" s="3">
+        <v>0.42580983135389999</v>
+      </c>
+      <c r="M64" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB64" s="3"/>
+      <c r="AC64" s="3"/>
+      <c r="AD64" s="3"/>
+      <c r="AE64" s="3"/>
+    </row>
+    <row r="65" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>76</v>
+      </c>
+      <c r="B65">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="C65">
+        <v>0.1</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>-0.2</v>
+      </c>
+      <c r="F65">
+        <v>0.1</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+      <c r="I65" s="3">
+        <v>0.18880473461709801</v>
+      </c>
+      <c r="J65" s="3">
+        <v>8.1890329798867106E-3</v>
+      </c>
+      <c r="K65" s="3">
+        <v>0.192274783519122</v>
+      </c>
+      <c r="L65" s="3">
+        <v>0.39037508165444401</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB65" s="3"/>
+      <c r="AC65" s="3"/>
+      <c r="AD65" s="3"/>
+      <c r="AE65" s="3"/>
+    </row>
+    <row r="66" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B66">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="C66">
+        <v>0.1</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <v>-0.2</v>
+      </c>
+      <c r="F66">
+        <v>0.2</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+      <c r="I66" s="3">
+        <v>0.180675764457642</v>
+      </c>
+      <c r="J66" s="3">
+        <v>8.1019588135258901E-3</v>
+      </c>
+      <c r="K66" s="3">
+        <v>0.18653712115293999</v>
+      </c>
+      <c r="L66" s="3">
+        <v>0.374926803387721</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB66" s="3"/>
+      <c r="AC66" s="3"/>
+      <c r="AD66" s="3"/>
+      <c r="AE66" s="3"/>
+    </row>
+    <row r="67" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B67">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="C67">
+        <v>0.1</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>-0.2</v>
+      </c>
+      <c r="F67">
+        <v>0.3</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+      <c r="I67" s="3">
+        <v>0.173141956318067</v>
+      </c>
+      <c r="J67" s="3">
+        <v>8.0292745572652004E-3</v>
+      </c>
+      <c r="K67" s="3">
+        <v>0.181315209874674</v>
+      </c>
+      <c r="L67" s="3">
+        <v>0.362078485283231</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB67" s="3"/>
+      <c r="AC67" s="3"/>
+      <c r="AD67" s="3"/>
+      <c r="AE67" s="3"/>
+    </row>
+    <row r="68" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B68">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="C68">
+        <v>0.1</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>-0.2</v>
+      </c>
+      <c r="F68">
+        <v>0.5</v>
+      </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
+      <c r="I68" s="3">
+        <v>0.159633906306971</v>
+      </c>
+      <c r="J68" s="3">
+        <v>7.9229261478554695E-3</v>
+      </c>
+      <c r="K68" s="3">
+        <v>0.17047479097177401</v>
+      </c>
+      <c r="L68" s="3">
+        <v>0.33783072236714201</v>
+      </c>
+      <c r="Q68" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B69">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="C69">
+        <v>0.1</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>-0.2</v>
+      </c>
+      <c r="F69">
+        <v>0.8</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="I69" s="3">
+        <v>0.14247854311326399</v>
+      </c>
+      <c r="J69" s="3">
+        <v>7.8508707367145793E-3</v>
+      </c>
+      <c r="K69" s="3">
+        <v>0.15735585822027201</v>
+      </c>
+      <c r="L69" s="3">
+        <v>0.30389911218937299</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B70">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="C70">
+        <v>0.1</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <v>-0.2</v>
+      </c>
+      <c r="F70">
+        <v>1.5</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="I70" s="3">
+        <v>0.11414060246359201</v>
+      </c>
+      <c r="J70" s="3">
+        <v>8.0715675877402002E-3</v>
+      </c>
+      <c r="K70" s="3">
+        <v>0.13391984302920401</v>
+      </c>
+      <c r="L70" s="3">
+        <v>0.26862145135224602</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="71" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="B71">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="C71">
+        <v>0.1</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>-0.2</v>
+      </c>
+      <c r="F71">
+        <v>2</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+      <c r="I71" s="3">
+        <v>0.102055838712674</v>
+      </c>
+      <c r="J71" s="3">
+        <v>8.6592471265246902E-3</v>
+      </c>
+      <c r="K71" s="3">
+        <v>0.122982788932036</v>
+      </c>
+      <c r="L71" s="3">
+        <v>0.50189872779143996</v>
+      </c>
+      <c r="M71" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added in model 2 in same simulation
</commit_message>
<xml_diff>
--- a/Gainsheet.xlsx
+++ b/Gainsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hampu\Documents\Atmel Studio\7.0\AutoBike-Simulation-MDH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1921DF60-C078-40DF-920F-6BCA88913A99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE5FEFBE-D7D1-41CC-8393-FB8782257AB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="88">
   <si>
     <t>I Lat</t>
   </si>
@@ -243,27 +243,6 @@
     <t>Okey that is to much</t>
   </si>
   <si>
-    <t>Seem to be able to scale just lateral gain</t>
-  </si>
-  <si>
-    <t>Best</t>
-  </si>
-  <si>
-    <t>0.25 phead is unstable</t>
-  </si>
-  <si>
-    <t>unstable</t>
-  </si>
-  <si>
-    <t>not better</t>
-  </si>
-  <si>
-    <t>Integration on heading</t>
-  </si>
-  <si>
-    <t>Ocsillation in rrt</t>
-  </si>
-  <si>
     <t>Init 40d yaw</t>
   </si>
   <si>
@@ -307,6 +286,12 @@
   </si>
   <si>
     <t xml:space="preserve">Might finish but won't is not stable </t>
+  </si>
+  <si>
+    <t>Lean angles on 30 degrees and overshoots</t>
+  </si>
+  <si>
+    <t>Disturbance</t>
   </si>
 </sst>
 </file>
@@ -2500,8 +2485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B706E9A-D8F2-483B-90DB-055EAB945C48}">
   <dimension ref="A1:AE75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:L1"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="I63" sqref="I63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2557,7 +2542,7 @@
         <v>9</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="R1" s="3" t="s">
         <v>8</v>
@@ -3315,7 +3300,7 @@
         <v>1.1642512996067</v>
       </c>
       <c r="W23" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="Y23" s="5">
         <v>2.26901864123771</v>
@@ -3362,7 +3347,7 @@
         <v>1.0560991687771699</v>
       </c>
       <c r="W24" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.25">
@@ -4272,7 +4257,7 @@
         <v>0.69841633006716597</v>
       </c>
       <c r="W53" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="AB53" s="3"/>
       <c r="AC53" s="3"/>
@@ -4625,17 +4610,18 @@
       <c r="AE62" s="3"/>
     </row>
     <row r="63" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B63">
-        <v>8.5</v>
-      </c>
-      <c r="C63">
+      <c r="A63" s="3"/>
+      <c r="B63" s="3">
+        <v>7</v>
+      </c>
+      <c r="C63" s="3">
         <v>0.1</v>
       </c>
-      <c r="D63">
+      <c r="D63" s="3">
         <v>0</v>
       </c>
       <c r="E63">
-        <v>-0.2</v>
+        <v>-0.3</v>
       </c>
       <c r="F63">
         <v>0</v>
@@ -4643,498 +4629,179 @@
       <c r="G63">
         <v>0</v>
       </c>
-      <c r="I63" s="3">
-        <v>0.20531231897257701</v>
-      </c>
-      <c r="J63" s="3">
-        <v>8.2103376639326795E-3</v>
-      </c>
-      <c r="K63" s="3">
-        <v>0.20613832476131999</v>
-      </c>
-      <c r="L63" s="3">
-        <v>0.42158025194620702</v>
-      </c>
-      <c r="M63" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q63" t="s">
+      <c r="I63"/>
+      <c r="J63"/>
+      <c r="M63" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="AB63" s="3"/>
-      <c r="AC63" s="3"/>
-      <c r="AD63" s="3"/>
-      <c r="AE63" s="3"/>
+      <c r="N63" s="3"/>
+      <c r="R63"/>
+      <c r="S63"/>
+      <c r="T63"/>
+      <c r="U63"/>
     </row>
     <row r="64" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B64">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="C64">
-        <v>0.1</v>
-      </c>
-      <c r="D64">
-        <v>0</v>
-      </c>
-      <c r="E64">
-        <v>-0.2</v>
-      </c>
-      <c r="F64">
-        <v>0</v>
-      </c>
-      <c r="G64">
-        <v>0</v>
-      </c>
-      <c r="I64" s="3">
-        <v>0.19788991614684101</v>
-      </c>
-      <c r="J64" s="3">
-        <v>8.2918695558750095E-3</v>
-      </c>
-      <c r="K64" s="3">
-        <v>0.19913233611959399</v>
-      </c>
-      <c r="L64" s="3">
-        <v>0.40535708876434501</v>
-      </c>
-      <c r="N64" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q64" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB64" s="3"/>
-      <c r="AC64" s="3"/>
-      <c r="AD64" s="3"/>
-      <c r="AE64" s="3"/>
-    </row>
-    <row r="65" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B65">
-        <v>8.9</v>
-      </c>
-      <c r="C65">
-        <v>0.1</v>
-      </c>
-      <c r="D65">
-        <v>0</v>
-      </c>
-      <c r="E65">
-        <v>-0.2</v>
-      </c>
-      <c r="F65">
-        <v>0</v>
-      </c>
-      <c r="G65">
-        <v>0</v>
-      </c>
-      <c r="I65" s="3">
-        <v>0.19547645074810199</v>
-      </c>
-      <c r="J65" s="3">
-        <v>8.3551382640506197E-3</v>
-      </c>
-      <c r="K65" s="3">
-        <v>0.19673082710140799</v>
-      </c>
-      <c r="L65" s="3">
-        <v>0.39266440377241602</v>
-      </c>
-      <c r="Q65" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB65" s="3"/>
-      <c r="AC65" s="3"/>
-      <c r="AD65" s="3"/>
-      <c r="AE65" s="3"/>
-    </row>
-    <row r="66" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B66">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="C66">
-        <v>0.1</v>
-      </c>
-      <c r="D66">
-        <v>0</v>
-      </c>
-      <c r="E66">
-        <v>-0.15</v>
-      </c>
-      <c r="F66">
-        <v>0</v>
-      </c>
-      <c r="G66">
-        <v>0</v>
-      </c>
-      <c r="I66" s="3">
-        <v>0.217646255171216</v>
-      </c>
-      <c r="J66" s="3">
-        <v>9.2268067433461508E-3</v>
-      </c>
-      <c r="K66" s="3">
-        <v>0.209649118587137</v>
-      </c>
-      <c r="L66" s="3">
-        <v>0.44740215370637199</v>
-      </c>
-      <c r="M66" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q66" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB66" s="3"/>
-      <c r="AC66" s="3"/>
-      <c r="AD66" s="3"/>
-      <c r="AE66" s="3"/>
-    </row>
-    <row r="67" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B67">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="C67">
-        <v>0.1</v>
-      </c>
-      <c r="D67">
-        <v>0.05</v>
-      </c>
-      <c r="E67">
-        <v>-0.2</v>
-      </c>
-      <c r="F67">
-        <v>0</v>
-      </c>
-      <c r="G67">
-        <v>0</v>
-      </c>
-      <c r="I67" s="3">
-        <v>4.6638026290516903</v>
-      </c>
-      <c r="J67" s="3">
-        <v>6.06937780118544</v>
-      </c>
-      <c r="K67" s="3">
-        <v>10.8314863409102</v>
-      </c>
-      <c r="L67" s="3">
-        <v>6.7123885481414201</v>
-      </c>
-      <c r="M67" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q67" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB67" s="3"/>
-      <c r="AC67" s="3"/>
-      <c r="AD67" s="3"/>
-      <c r="AE67" s="3"/>
-    </row>
-    <row r="68" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B68">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="C68">
-        <v>0.1</v>
-      </c>
-      <c r="D68">
-        <v>-0.05</v>
-      </c>
-      <c r="E68">
-        <v>-0.2</v>
-      </c>
-      <c r="F68">
-        <v>0</v>
-      </c>
-      <c r="G68">
-        <v>0</v>
-      </c>
-      <c r="I68" s="3">
-        <v>0.20650916723489801</v>
-      </c>
-      <c r="J68" s="3">
-        <v>8.4180547425808192E-3</v>
-      </c>
-      <c r="K68" s="3">
-        <v>0.204775763364448</v>
-      </c>
-      <c r="L68" s="3">
-        <v>0.42580983135389999</v>
-      </c>
-      <c r="M68" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q68" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB68" s="3"/>
-      <c r="AC68" s="3"/>
-      <c r="AD68" s="3"/>
-      <c r="AE68" s="3"/>
-    </row>
-    <row r="69" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>76</v>
-      </c>
-      <c r="B69">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="C69">
-        <v>0.1</v>
-      </c>
-      <c r="D69">
-        <v>0</v>
-      </c>
-      <c r="E69">
-        <v>-0.2</v>
-      </c>
-      <c r="F69">
-        <v>0.1</v>
-      </c>
-      <c r="G69">
-        <v>0</v>
-      </c>
-      <c r="I69" s="3">
-        <v>0.18880473461709801</v>
-      </c>
-      <c r="J69" s="3">
-        <v>8.1890329798867106E-3</v>
-      </c>
-      <c r="K69" s="3">
-        <v>0.192274783519122</v>
-      </c>
-      <c r="L69" s="3">
-        <v>0.39037508165444401</v>
-      </c>
-      <c r="Q69" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB69" s="3"/>
-      <c r="AC69" s="3"/>
-      <c r="AD69" s="3"/>
-      <c r="AE69" s="3"/>
-    </row>
-    <row r="70" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B70">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="C70">
-        <v>0.1</v>
-      </c>
-      <c r="D70">
-        <v>0</v>
-      </c>
-      <c r="E70">
-        <v>-0.2</v>
-      </c>
-      <c r="F70">
-        <v>0.2</v>
-      </c>
-      <c r="G70">
-        <v>0</v>
-      </c>
-      <c r="I70" s="3">
-        <v>0.180675764457642</v>
-      </c>
-      <c r="J70" s="3">
-        <v>8.1019588135258901E-3</v>
-      </c>
-      <c r="K70" s="3">
-        <v>0.18653712115293999</v>
-      </c>
-      <c r="L70" s="3">
-        <v>0.374926803387721</v>
-      </c>
-      <c r="Q70" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB70" s="3"/>
-      <c r="AC70" s="3"/>
-      <c r="AD70" s="3"/>
-      <c r="AE70" s="3"/>
-    </row>
-    <row r="71" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B71">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="C71">
-        <v>0.1</v>
-      </c>
-      <c r="D71">
-        <v>0</v>
-      </c>
-      <c r="E71">
-        <v>-0.2</v>
-      </c>
-      <c r="F71">
-        <v>0.3</v>
-      </c>
-      <c r="G71">
-        <v>0</v>
-      </c>
-      <c r="I71" s="3">
-        <v>0.173141956318067</v>
-      </c>
-      <c r="J71" s="3">
-        <v>8.0292745572652004E-3</v>
-      </c>
-      <c r="K71" s="3">
-        <v>0.181315209874674</v>
-      </c>
-      <c r="L71" s="3">
-        <v>0.362078485283231</v>
-      </c>
-      <c r="Q71" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB71" s="3"/>
-      <c r="AC71" s="3"/>
-      <c r="AD71" s="3"/>
-      <c r="AE71" s="3"/>
-    </row>
-    <row r="72" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B72">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="C72">
-        <v>0.1</v>
-      </c>
-      <c r="D72">
-        <v>0</v>
-      </c>
-      <c r="E72">
-        <v>-0.2</v>
-      </c>
-      <c r="F72">
-        <v>0.5</v>
-      </c>
-      <c r="G72">
-        <v>0</v>
-      </c>
-      <c r="I72" s="3">
-        <v>0.159633906306971</v>
-      </c>
-      <c r="J72" s="3">
-        <v>7.9229261478554695E-3</v>
-      </c>
-      <c r="K72" s="3">
-        <v>0.17047479097177401</v>
-      </c>
-      <c r="L72" s="3">
-        <v>0.33783072236714201</v>
-      </c>
-      <c r="Q72" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="73" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B73">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="C73">
-        <v>0.1</v>
-      </c>
-      <c r="D73">
-        <v>0</v>
-      </c>
-      <c r="E73">
-        <v>-0.2</v>
-      </c>
-      <c r="F73">
-        <v>0.8</v>
-      </c>
-      <c r="G73">
-        <v>0</v>
-      </c>
-      <c r="I73" s="3">
-        <v>0.14247854311326399</v>
-      </c>
-      <c r="J73" s="3">
-        <v>7.8508707367145793E-3</v>
-      </c>
-      <c r="K73" s="3">
-        <v>0.15735585822027201</v>
-      </c>
-      <c r="L73" s="3">
-        <v>0.30389911218937299</v>
-      </c>
-      <c r="Q73" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="74" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B74">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="C74">
-        <v>0.1</v>
-      </c>
-      <c r="D74">
-        <v>0</v>
-      </c>
-      <c r="E74">
-        <v>-0.2</v>
-      </c>
-      <c r="F74">
-        <v>1.5</v>
-      </c>
-      <c r="G74">
-        <v>0</v>
-      </c>
-      <c r="I74" s="3">
-        <v>0.11414060246359201</v>
-      </c>
-      <c r="J74" s="3">
-        <v>8.0715675877402002E-3</v>
-      </c>
-      <c r="K74" s="3">
-        <v>0.13391984302920401</v>
-      </c>
-      <c r="L74" s="3">
-        <v>0.26862145135224602</v>
-      </c>
-      <c r="Q74" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="75" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B75">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="C75">
-        <v>0.1</v>
-      </c>
-      <c r="D75">
-        <v>0</v>
-      </c>
-      <c r="E75">
-        <v>-0.2</v>
-      </c>
-      <c r="F75">
-        <v>2</v>
-      </c>
-      <c r="G75">
-        <v>0</v>
-      </c>
-      <c r="I75" s="3">
-        <v>0.102055838712674</v>
-      </c>
-      <c r="J75" s="3">
-        <v>8.6592471265246902E-3</v>
-      </c>
-      <c r="K75" s="3">
-        <v>0.122982788932036</v>
-      </c>
-      <c r="L75" s="3">
-        <v>0.50189872779143996</v>
-      </c>
-      <c r="M75" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q75" t="s">
-        <v>67</v>
-      </c>
+      <c r="A64" s="3"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="I64"/>
+      <c r="J64"/>
+      <c r="M64" s="3"/>
+      <c r="N64" s="3"/>
+      <c r="R64"/>
+      <c r="S64"/>
+      <c r="T64"/>
+      <c r="U64"/>
+    </row>
+    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A65" s="3"/>
+      <c r="M65" s="3"/>
+      <c r="N65" s="3"/>
+      <c r="R65"/>
+      <c r="S65"/>
+      <c r="T65"/>
+      <c r="U65"/>
+    </row>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A66" s="3"/>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="I66"/>
+      <c r="J66"/>
+      <c r="M66" s="3"/>
+      <c r="N66" s="3"/>
+      <c r="R66"/>
+      <c r="S66"/>
+      <c r="T66"/>
+      <c r="U66"/>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A67" s="3"/>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="I67"/>
+      <c r="J67"/>
+      <c r="M67" s="3"/>
+      <c r="N67" s="3"/>
+      <c r="R67"/>
+      <c r="S67"/>
+      <c r="T67"/>
+      <c r="U67"/>
+    </row>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A68" s="3"/>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="I68"/>
+      <c r="J68"/>
+      <c r="M68" s="3"/>
+      <c r="N68" s="3"/>
+      <c r="R68"/>
+      <c r="S68"/>
+      <c r="T68"/>
+      <c r="U68"/>
+    </row>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A69" s="3"/>
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="I69"/>
+      <c r="J69"/>
+      <c r="M69" s="3"/>
+      <c r="N69" s="3"/>
+      <c r="R69"/>
+      <c r="S69"/>
+      <c r="T69"/>
+      <c r="U69"/>
+    </row>
+    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A70" s="3"/>
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="I70"/>
+      <c r="J70"/>
+      <c r="M70" s="3"/>
+      <c r="N70" s="3"/>
+      <c r="R70"/>
+      <c r="S70"/>
+      <c r="T70"/>
+      <c r="U70"/>
+    </row>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A71" s="3"/>
+      <c r="B71" s="3"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="I71"/>
+      <c r="J71"/>
+      <c r="M71" s="3"/>
+      <c r="N71" s="3"/>
+      <c r="R71"/>
+      <c r="S71"/>
+      <c r="T71"/>
+      <c r="U71"/>
+    </row>
+    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A72" s="3"/>
+      <c r="B72" s="3"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="I72"/>
+      <c r="J72"/>
+      <c r="K72"/>
+      <c r="L72"/>
+      <c r="R72"/>
+      <c r="S72"/>
+      <c r="T72"/>
+      <c r="U72"/>
+    </row>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A73" s="3"/>
+      <c r="B73" s="3"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="I73"/>
+      <c r="J73"/>
+      <c r="K73"/>
+      <c r="L73"/>
+      <c r="R73"/>
+      <c r="S73"/>
+      <c r="T73"/>
+      <c r="U73"/>
+    </row>
+    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A74" s="3"/>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="I74"/>
+      <c r="J74"/>
+      <c r="K74"/>
+      <c r="L74"/>
+      <c r="R74"/>
+      <c r="S74"/>
+      <c r="T74"/>
+      <c r="U74"/>
+    </row>
+    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A75" s="3"/>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="I75"/>
+      <c r="J75"/>
+      <c r="K75"/>
+      <c r="L75"/>
+      <c r="R75"/>
+      <c r="S75"/>
+      <c r="T75"/>
+      <c r="U75"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5147,7 +4814,7 @@
   <dimension ref="B1:Q63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+      <selection activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5187,6 +4854,9 @@
       <c r="L1" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="O1" s="3" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2">
@@ -5284,7 +4954,7 @@
         <v>2.0927196091165401</v>
       </c>
       <c r="P4" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
@@ -5319,10 +4989,10 @@
         <v>1.8045168286751201</v>
       </c>
       <c r="M5" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="P5" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
@@ -5357,13 +5027,13 @@
         <v>1.6661450589256099</v>
       </c>
       <c r="M6" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="P6" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="Q6" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
@@ -5558,10 +5228,10 @@
         <v>1.28777287133427</v>
       </c>
       <c r="N12" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="Q12" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
@@ -5596,10 +5266,10 @@
         <v>1.12420468065956</v>
       </c>
       <c r="N13" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="Q13" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.25">
@@ -5698,7 +5368,7 @@
         <v>0.62649289478592296</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>15</v>
       </c>
@@ -5729,8 +5399,11 @@
       <c r="L17" s="3">
         <v>0.54025141496027396</v>
       </c>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="O17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>18</v>
       </c>
@@ -5762,7 +5435,7 @@
         <v>0.478304981914496</v>
       </c>
     </row>
-    <row r="19" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>20</v>
       </c>
@@ -5794,10 +5467,10 @@
         <v>5.9331618756728801</v>
       </c>
       <c r="M19" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>18</v>
       </c>
@@ -5829,10 +5502,10 @@
         <v>7.4786645283351199</v>
       </c>
       <c r="M20" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>18</v>
       </c>
@@ -5864,10 +5537,10 @@
         <v>0.505817784664092</v>
       </c>
       <c r="N21" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>18</v>
       </c>
@@ -5899,7 +5572,7 @@
         <v>0.49361691946678499</v>
       </c>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>18</v>
       </c>
@@ -5931,7 +5604,7 @@
         <v>0.50462346682550796</v>
       </c>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>18</v>
       </c>
@@ -5963,7 +5636,7 @@
         <v>0.46338719534004302</v>
       </c>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>18</v>
       </c>
@@ -5995,10 +5668,10 @@
         <v>0.47825470190924702</v>
       </c>
       <c r="M25" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>18</v>
       </c>
@@ -6030,40 +5703,69 @@
         <v>0.47687954156482099</v>
       </c>
       <c r="M26" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
-    </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B29" s="3">
+        <v>7</v>
+      </c>
+      <c r="C29" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>-0.2</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>1.3394385231052399</v>
+      </c>
+      <c r="J29">
+        <v>1.19611140272806E-2</v>
+      </c>
+      <c r="K29" s="3">
+        <v>0.98415136500439404</v>
+      </c>
+      <c r="L29" s="3">
+        <v>2.1725513596830801</v>
+      </c>
+      <c r="N29" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>

</xml_diff>

<commit_message>
Updated gains and new model 1 calc
</commit_message>
<xml_diff>
--- a/Gainsheet.xlsx
+++ b/Gainsheet.xlsx
@@ -8,26 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hampu\Documents\Atmel Studio\7.0\AutoBike-Simulation-MDH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE5FEFBE-D7D1-41CC-8393-FB8782257AB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7B4C86-1226-402B-8B90-27BB2D12943E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="99">
   <si>
     <t>I Lat</t>
   </si>
@@ -292,6 +301,39 @@
   </si>
   <si>
     <t>Disturbance</t>
+  </si>
+  <si>
+    <t>14km</t>
+  </si>
+  <si>
+    <t>10km safe</t>
+  </si>
+  <si>
+    <t>Enkel kin stabil</t>
+  </si>
+  <si>
+    <t>Safe MDH kin</t>
+  </si>
+  <si>
+    <t>Aggressiv MDH kin</t>
+  </si>
+  <si>
+    <t>Log2</t>
+  </si>
+  <si>
+    <t>run 700 speed</t>
+  </si>
+  <si>
+    <t>Saturation test</t>
+  </si>
+  <si>
+    <t>10k safe balancing. Drive straight and turn back yaw test, try lateral+heading angle wonky</t>
+  </si>
+  <si>
+    <t>14k balancing</t>
+  </si>
+  <si>
+    <t>10km agressive</t>
   </si>
 </sst>
 </file>
@@ -629,7 +671,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
@@ -2482,11 +2524,177 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C42746-A18A-44E9-B216-8A75560B9333}">
+  <dimension ref="A1:L8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="82.28515625" customWidth="1"/>
+    <col min="13" max="16" width="44.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K1">
+        <v>6</v>
+      </c>
+      <c r="L1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2">
+        <v>3.4180000000000001</v>
+      </c>
+      <c r="C2">
+        <f>60/1.327</f>
+        <v>45.214770158251696</v>
+      </c>
+      <c r="D2">
+        <f>0.0646/60</f>
+        <v>1.0766666666666667E-3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>94</v>
+      </c>
+      <c r="K2">
+        <v>7</v>
+      </c>
+      <c r="L2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3">
+        <v>4.8048999999999999</v>
+      </c>
+      <c r="C3">
+        <f>60/1.1908</f>
+        <v>50.386294927779637</v>
+      </c>
+      <c r="D3">
+        <f>0.0566/60</f>
+        <v>9.4333333333333324E-4</v>
+      </c>
+      <c r="K3">
+        <v>8</v>
+      </c>
+      <c r="L3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4">
+        <v>5.7843999999999998</v>
+      </c>
+      <c r="C4">
+        <f>60/1.6066</f>
+        <v>37.345947964645838</v>
+      </c>
+      <c r="D4">
+        <f>0.0545/60</f>
+        <v>9.0833333333333337E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <f>60/0.1</f>
+        <v>600</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>-0.2</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <f>60/0.2</f>
+        <v>300</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>-0.8</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <f>60/0.2</f>
+        <v>300</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>-1</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B706E9A-D8F2-483B-90DB-055EAB945C48}">
   <dimension ref="A1:AE75"/>
   <sheetViews>
     <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="I63" sqref="I63"/>
+      <selection activeCell="B52" sqref="B52:G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4809,12 +5017,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EA8A450-1403-471B-B170-D70336124AE8}">
   <dimension ref="B1:Q63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q29" sqref="Q29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>